<commit_message>
Add fitur Menu Supplier
</commit_message>
<xml_diff>
--- a/POS/public/template_supplier.xlsx
+++ b/POS/public/template_supplier.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/PWL_2025/week8/PWL_POS/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/PWL_2025/POS/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0588A1-526F-5848-A966-ABB37B0EB2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6ED98FA-599B-F740-A732-55601C19F250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21760" yWindow="5720" windowWidth="11600" windowHeight="7160" xr2:uid="{F4AF122A-7E61-DF45-99C0-90FDA8B5C785}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>supplier_id</t>
   </si>
@@ -45,9 +45,6 @@
     <t>supplier_nama</t>
   </si>
   <si>
-    <t>supplier_telp</t>
-  </si>
-  <si>
     <t>supplier_alamat</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
   </si>
   <si>
     <t>PT Testing</t>
-  </si>
-  <si>
-    <t>021-123654</t>
   </si>
   <si>
     <t>Jl. Soekarno Hatta, No. 13, Malang</t>
@@ -412,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD6B5297-0787-4B4E-87B6-EA2172849EC7}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -426,7 +420,7 @@
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,25 +433,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>